<commit_message>
le bon commit de fin de semaine ^^
</commit_message>
<xml_diff>
--- a/linux_glossaire.xlsx
+++ b/linux_glossaire.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="123">
   <si>
     <t>Commande</t>
   </si>
@@ -243,9 +243,6 @@
     <t>up / down (éteindre/allumer/interface)</t>
   </si>
   <si>
-    <t>permet de modifier qsa configuration réseau</t>
-  </si>
-  <si>
     <t>man</t>
   </si>
   <si>
@@ -309,9 +306,6 @@
     <t>grep [mot à rechercher]</t>
   </si>
   <si>
-    <t>chercher un mot dans des fichiers</t>
-  </si>
-  <si>
     <t>"super utilisateur do": excécuter une commande avec les droits d'admin (élevation de privilèges)</t>
   </si>
   <si>
@@ -327,9 +321,6 @@
     <t>"move": déplacer un fichier de dossier / renommer un fichier</t>
   </si>
   <si>
-    <t>mw [fichier/dossier][destination][nouveau nom]</t>
-  </si>
-  <si>
     <t>rmdir -p (supp arborescence)</t>
   </si>
   <si>
@@ -352,6 +343,51 @@
   </si>
   <si>
     <t>packet internet groper</t>
+  </si>
+  <si>
+    <t>permet de modifier sa configuration réseau</t>
+  </si>
+  <si>
+    <t>supprimer un utilisateur</t>
+  </si>
+  <si>
+    <t>créer un groupe</t>
+  </si>
+  <si>
+    <t>groupadd</t>
+  </si>
+  <si>
+    <t>chown</t>
+  </si>
+  <si>
+    <t>change le propriétaire</t>
+  </si>
+  <si>
+    <t>chmod</t>
+  </si>
+  <si>
+    <t>change les droits</t>
+  </si>
+  <si>
+    <t>deluser</t>
+  </si>
+  <si>
+    <t>deluser [nom][groupe]</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> -R</t>
+  </si>
+  <si>
+    <t>passwd</t>
+  </si>
+  <si>
+    <t>changer le mot de passe</t>
+  </si>
+  <si>
+    <t>find / -name</t>
+  </si>
+  <si>
+    <t>chercher un mot dans des fichiers / actualiser date pub</t>
   </si>
 </sst>
 </file>
@@ -793,10 +829,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D38"/>
+  <dimension ref="A1:D44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
+    <sheetView tabSelected="1" topLeftCell="C19" workbookViewId="0">
+      <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -858,7 +894,7 @@
         <v>35</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -981,7 +1017,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
         <v>11</v>
       </c>
@@ -1060,7 +1096,9 @@
         <v>24</v>
       </c>
       <c r="B21" s="9"/>
-      <c r="C21" s="9"/>
+      <c r="C21" s="9" t="s">
+        <v>101</v>
+      </c>
       <c r="D21" s="10" t="s">
         <v>67</v>
       </c>
@@ -1126,134 +1164,188 @@
       </c>
       <c r="C27" s="9"/>
       <c r="D27" s="10" t="s">
-        <v>74</v>
+        <v>108</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="C28" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="C28" s="12" t="s">
+      <c r="D28" s="13" t="s">
         <v>76</v>
-      </c>
-      <c r="D28" s="13" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="11" t="s">
-        <v>78</v>
-      </c>
-      <c r="C29" s="12" t="s">
-        <v>102</v>
+        <v>77</v>
       </c>
       <c r="D29" s="13" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="B30" s="12" t="s">
         <v>79</v>
       </c>
-      <c r="B30" s="12" t="s">
+      <c r="D30" s="13" t="s">
         <v>80</v>
-      </c>
-      <c r="D30" s="13" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="C31" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="C31" s="12" t="s">
+      <c r="D31" s="13" t="s">
         <v>83</v>
-      </c>
-      <c r="D31" s="13" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="B32" s="12" t="s">
         <v>85</v>
       </c>
-      <c r="B32" s="12" t="s">
+      <c r="C32" s="12" t="s">
         <v>86</v>
       </c>
-      <c r="C32" s="12" t="s">
+      <c r="D32" s="13" t="s">
         <v>87</v>
-      </c>
-      <c r="D32" s="13" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="11" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B33" s="12" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="C33" s="12" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="D33" s="13" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="B34" s="12" t="s">
         <v>90</v>
       </c>
-      <c r="B34" s="12" t="s">
+      <c r="D34" s="13" t="s">
         <v>91</v>
-      </c>
-      <c r="D34" s="13" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="B35" s="12" t="s">
         <v>93</v>
       </c>
-      <c r="B35" s="12" t="s">
+      <c r="C35" s="12" t="s">
         <v>94</v>
       </c>
-      <c r="C35" s="12" t="s">
-        <v>95</v>
-      </c>
       <c r="D35" s="13" t="s">
-        <v>96</v>
+        <v>122</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="11" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D36" s="13" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="B37" s="12" t="s">
         <v>100</v>
       </c>
-      <c r="B37" s="12" t="s">
-        <v>103</v>
-      </c>
       <c r="C37" s="12" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="D37" s="13" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="11" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="D38" s="13" t="s">
-        <v>107</v>
+        <v>104</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="C39" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="D39" s="13" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="11" t="s">
+        <v>111</v>
+      </c>
+      <c r="D40" s="13" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="B41" s="12" t="s">
+        <v>118</v>
+      </c>
+      <c r="D41" s="13" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="B42" s="12" t="s">
+        <v>118</v>
+      </c>
+      <c r="D42" s="13" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="11" t="s">
+        <v>119</v>
+      </c>
+      <c r="D43" s="13" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="C44" s="12" t="s">
+        <v>121</v>
       </c>
     </row>
   </sheetData>

</xml_diff>